<commit_message>
adição da figura g.10 - validar com wagner
</commit_message>
<xml_diff>
--- a/Data/g1.9.xlsx
+++ b/Data/g1.9.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>Período</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Categoria</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -461,7 +466,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Todos os anos</t>
+          <t>2010 / 2022</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Toda a série histórica</t>
         </is>
       </c>
     </row>
@@ -476,7 +486,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Todos os anos</t>
+          <t>2010 / 2022</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Toda a série histórica</t>
         </is>
       </c>
     </row>
@@ -491,7 +506,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Todos os anos</t>
+          <t>2010 / 2022</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Toda a série histórica</t>
         </is>
       </c>
     </row>
@@ -506,7 +526,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Todos os anos</t>
+          <t>2010 / 2022</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Toda a série histórica</t>
         </is>
       </c>
     </row>
@@ -521,7 +546,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Todos os anos</t>
+          <t>2010 / 2022</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Toda a série histórica</t>
         </is>
       </c>
     </row>
@@ -536,7 +566,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Todos os anos</t>
+          <t>2010 / 2022</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Toda a série histórica</t>
         </is>
       </c>
     </row>
@@ -551,7 +586,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Último ano</t>
+          <t>2021 / 2022</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Último ano da série histórica</t>
         </is>
       </c>
     </row>
@@ -566,7 +606,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Último ano</t>
+          <t>2021 / 2022</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Último ano da série histórica</t>
         </is>
       </c>
     </row>
@@ -581,7 +626,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Último ano</t>
+          <t>2021 / 2022</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Último ano da série histórica</t>
         </is>
       </c>
     </row>
@@ -596,7 +646,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Último ano</t>
+          <t>2021 / 2022</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Último ano da série histórica</t>
         </is>
       </c>
     </row>
@@ -611,7 +666,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Último ano</t>
+          <t>2021 / 2022</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Último ano da série histórica</t>
         </is>
       </c>
     </row>
@@ -626,7 +686,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Último ano</t>
+          <t>2021 / 2022</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Último ano da série histórica</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
g1.9 - ajuste na estrutura e cálculo da tabela
</commit_message>
<xml_diff>
--- a/Data/g1.9.xlsx
+++ b/Data/g1.9.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,11 +449,6 @@
           <t>Período</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Categoria</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -462,16 +457,11 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>49.99810519852372</v>
+        <v>35.19143837025082</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2010 / 2022</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Toda a série histórica</t>
+          <t>2012 / 2022</t>
         </is>
       </c>
     </row>
@@ -482,16 +472,11 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>39.08151956088085</v>
+        <v>31.76377306549257</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2010 / 2022</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Toda a série histórica</t>
+          <t>2012 / 2022</t>
         </is>
       </c>
     </row>
@@ -502,36 +487,26 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>27.7784463299374</v>
+        <v>21.77658698762782</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2010 / 2022</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Toda a série histórica</t>
+          <t>2012 / 2022</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Eletricidade e gás, água, esgoto, atividades de gestão de resíduos e descontaminação</t>
+          <t>Agropecuária</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>16.19046508148367</v>
+        <v>9.730306427073359</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2010 / 2022</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Toda a série histórica</t>
+          <t>2012 / 2022</t>
         </is>
       </c>
     </row>
@@ -542,36 +517,26 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6.827240591078635</v>
+        <v>4.760483082368495</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2010 / 2022</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Toda a série histórica</t>
+          <t>2012 / 2022</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Agropecuária</t>
+          <t>Eletricidade e gás, água, esgoto, atividades de gestão de resíduos e descontaminação</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-6.117221074957826</v>
+        <v>2.412539862254022</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2010 / 2022</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Toda a série histórica</t>
+          <t>2012 / 2022</t>
         </is>
       </c>
     </row>
@@ -589,11 +554,6 @@
           <t>2021 / 2022</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Último ano da série histórica</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -609,11 +569,6 @@
           <t>2021 / 2022</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Último ano da série histórica</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -629,11 +584,6 @@
           <t>2021 / 2022</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Último ano da série histórica</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -649,11 +599,6 @@
           <t>2021 / 2022</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Último ano da série histórica</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -669,11 +614,6 @@
           <t>2021 / 2022</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Último ano da série histórica</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -687,11 +627,6 @@
       <c r="C13" t="inlineStr">
         <is>
           <t>2021 / 2022</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Último ano da série histórica</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
g1.9 - ajuste na coluna período para não inserir valor dinâmico
</commit_message>
<xml_diff>
--- a/Data/g1.9.xlsx
+++ b/Data/g1.9.xlsx
@@ -453,180 +453,180 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Atividades financeiras, de seguros e serviços relacionados</t>
+          <t>Transporte, armazenagem e correio</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>35.19143837025082</v>
+        <v>17.77773366884247</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2012 / 2022</t>
+          <t>atual/ano anterior</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Atividades imobiliárias</t>
+          <t>Agropecuária</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>31.76377306549257</v>
+        <v>6.521894003851491</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2012 / 2022</t>
+          <t>atual/ano anterior</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Informação e comunicação</t>
+          <t>Construção</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>21.77658698762782</v>
+        <v>6.438360842135382</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2012 / 2022</t>
+          <t>atual/ano anterior</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Agropecuária</t>
+          <t>Informação e comunicação</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>9.730306427073359</v>
+        <v>4.037854550070413</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2012 / 2022</t>
+          <t>atual/ano anterior</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Administração, defesa, educação e saúde públicas e seguridade social</t>
+          <t>Atividades imobiliárias</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.760483082368495</v>
+        <v>3.551068180916705</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2012 / 2022</t>
+          <t>atual/ano anterior</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Eletricidade e gás, água, esgoto, atividades de gestão de resíduos e descontaminação</t>
+          <t>Administração, defesa, educação e saúde públicas e seguridade social</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.412539862254022</v>
+        <v>1.274864519824148</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2012 / 2022</t>
+          <t>atual/ano anterior</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Transporte, armazenagem e correio</t>
+          <t>Atividades financeiras, de seguros e serviços relacionados</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17.77773366884247</v>
+        <v>35.19143837025082</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2021 / 2022</t>
+          <t>atual/dez anos antes</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Agropecuária</t>
+          <t>Atividades imobiliárias</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6.521894003851491</v>
+        <v>31.76377306549257</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2021 / 2022</t>
+          <t>atual/dez anos antes</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Construção</t>
+          <t>Informação e comunicação</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>6.438360842135382</v>
+        <v>21.77658698762782</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2021 / 2022</t>
+          <t>atual/dez anos antes</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Informação e comunicação</t>
+          <t>Agropecuária</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4.037854550070413</v>
+        <v>9.730306427073359</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2021 / 2022</t>
+          <t>atual/dez anos antes</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Atividades imobiliárias</t>
+          <t>Administração, defesa, educação e saúde públicas e seguridade social</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3.551068180916705</v>
+        <v>4.760483082368495</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2021 / 2022</t>
+          <t>atual/dez anos antes</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Administração, defesa, educação e saúde públicas e seguridade social</t>
+          <t>Eletricidade e gás, água, esgoto, atividades de gestão de resíduos e descontaminação</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1.274864519824148</v>
+        <v>2.412539862254022</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2021 / 2022</t>
+          <t>atual/dez anos antes</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
g1.9 - adição de categoria com valores fixos para uso no bi
</commit_message>
<xml_diff>
--- a/Data/g1.9.xlsx
+++ b/Data/g1.9.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,184 +449,249 @@
           <t>Período</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Categoria</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Transporte, armazenagem e correio</t>
+          <t>Atividades financeiras, de seguros e serviços relacionados</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17.77773366884247</v>
+        <v>35.19143837025082</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>atual/ano anterior</t>
+          <t>2012 / 2022</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Agropecuária</t>
+          <t>Atividades imobiliárias</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.521894003851491</v>
+        <v>31.76377306549257</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>atual/ano anterior</t>
+          <t>2012 / 2022</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Construção</t>
+          <t>Informação e comunicação</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.438360842135382</v>
+        <v>21.77658698762782</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>atual/ano anterior</t>
+          <t>2012 / 2022</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Informação e comunicação</t>
+          <t>Agropecuária</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4.037854550070413</v>
+        <v>9.730306427073359</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>atual/ano anterior</t>
+          <t>2012 / 2022</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Atividades imobiliárias</t>
+          <t>Administração, defesa, educação e saúde públicas e seguridade social</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.551068180916705</v>
+        <v>4.760483082368495</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>atual/ano anterior</t>
+          <t>2012 / 2022</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Administração, defesa, educação e saúde públicas e seguridade social</t>
+          <t>Eletricidade e gás, água, esgoto, atividades de gestão de resíduos e descontaminação</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.274864519824148</v>
+        <v>2.412539862254022</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>atual/ano anterior</t>
+          <t>2012 / 2022</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Atividades financeiras, de seguros e serviços relacionados</t>
+          <t>Transporte, armazenagem e correio</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>35.19143837025082</v>
+        <v>17.77773366884247</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>atual/dez anos antes</t>
+          <t>2021 / 2022</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Atividades imobiliárias</t>
+          <t>Agropecuária</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>31.76377306549257</v>
+        <v>6.521894003851491</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>atual/dez anos antes</t>
+          <t>2021 / 2022</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Informação e comunicação</t>
+          <t>Construção</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>21.77658698762782</v>
+        <v>6.438360842135382</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>atual/dez anos antes</t>
+          <t>2021 / 2022</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Agropecuária</t>
+          <t>Informação e comunicação</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>9.730306427073359</v>
+        <v>4.037854550070413</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>atual/dez anos antes</t>
+          <t>2021 / 2022</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Administração, defesa, educação e saúde públicas e seguridade social</t>
+          <t>Atividades imobiliárias</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4.760483082368495</v>
+        <v>3.551068180916705</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>atual/dez anos antes</t>
+          <t>2021 / 2022</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Eletricidade e gás, água, esgoto, atividades de gestão de resíduos e descontaminação</t>
+          <t>Administração, defesa, educação e saúde públicas e seguridade social</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2.412539862254022</v>
+        <v>1.274864519824148</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>atual/dez anos antes</t>
+          <t>2021 / 2022</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
g1.9 - atualização na filtragem de ano e remoção da coluna categoria
</commit_message>
<xml_diff>
--- a/Data/g1.9.xlsx
+++ b/Data/g1.9.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,89 +449,64 @@
           <t>Período</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Categoria</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Atividades financeiras, de seguros e serviços relacionados</t>
+          <t>Eletricidade e gás, água, esgoto, atividades de gestão de resíduos e descontaminação</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>35.19143837025082</v>
+        <v>30.3618246924122</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2012 / 2022</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
+          <t>2013 / 2022</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Atividades imobiliárias</t>
+          <t>Atividades financeiras, de seguros e serviços relacionados</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>31.76377306549257</v>
+        <v>27.4933798284287</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2012 / 2022</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
+          <t>2013 / 2022</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Informação e comunicação</t>
+          <t>Atividades imobiliárias</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>21.77658698762782</v>
+        <v>23.40818553225802</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2012 / 2022</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
+          <t>2013 / 2022</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Agropecuária</t>
+          <t>Informação e comunicação</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>9.730306427073359</v>
+        <v>9.265557954021503</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2012 / 2022</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
+          <t>2013 / 2022</t>
         </is>
       </c>
     </row>
@@ -542,36 +517,26 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.760483082368495</v>
+        <v>2.709036955545471</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2012 / 2022</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
+          <t>2013 / 2022</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Eletricidade e gás, água, esgoto, atividades de gestão de resíduos e descontaminação</t>
+          <t>Agropecuária</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.412539862254022</v>
+        <v>-4.003418719932625</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2012 / 2022</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
+          <t>2013 / 2022</t>
         </is>
       </c>
     </row>
@@ -589,11 +554,6 @@
           <t>2021 / 2022</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -609,11 +569,6 @@
           <t>2021 / 2022</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -629,11 +584,6 @@
           <t>2021 / 2022</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -649,11 +599,6 @@
           <t>2021 / 2022</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -669,11 +614,6 @@
           <t>2021 / 2022</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -687,11 +627,6 @@
       <c r="C13" t="inlineStr">
         <is>
           <t>2021 / 2022</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
         </is>
       </c>
     </row>

</xml_diff>